<commit_message>
Added HyperbolicDistribution.xlsx to development folder
</commit_message>
<xml_diff>
--- a/img2d-generator/development/HyperbolicDistribution.xlsx
+++ b/img2d-generator/development/HyperbolicDistribution.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helaha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Eclipse\ws-comsystanj\comsystanj\img2d-generator\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7039875F-80BA-4BB1-A0C6-E395A3D2BFCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8643B7CD-8C09-431D-83F9-A4A45D05E134}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27300" windowHeight="11364" xr2:uid="{963DD0FA-F37E-46EB-A119-DFD0EB7A6A09}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>µ</t>
   </si>
@@ -36,22 +36,10 @@
     <t>beta</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
     <t>K1</t>
   </si>
   <si>
     <t>Hyperbolic</t>
-  </si>
-  <si>
-    <t>Hyperbolic normalized</t>
-  </si>
-  <si>
-    <t>Max</t>
   </si>
   <si>
     <t>ThicknessMax</t>
@@ -59,15 +47,46 @@
   <si>
     <t>Scaling [0, 1]</t>
   </si>
+  <si>
+    <t>Hyperbolic short</t>
+  </si>
+  <si>
+    <t>https://demonstrations.wolfram.com/HyperbolicDistribution/</t>
+  </si>
+  <si>
+    <t>https://reference.wolfram.com/language/ref/HyperbolicDistribution.html</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Hyperbolic_distribution</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>Näherung mit exp Funktion: Vorteil scaling von 0 -1 und auch ohne Skalierung möglich</t>
+  </si>
+  <si>
+    <t>"-alpha&lt;beta&lt;alpha"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,9 +112,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -114,684 +134,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Hyperbo</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>lic</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Tabelle1!$B$3:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.28835877333528559</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.89943824861494659</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0456320119399338</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.1506035329802264</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.9594633687371203</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14.767281530454278</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>26.814839298194407</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>47.964457405949112</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>84.851081412184911</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>148.83916839835646</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F496-420F-9FFF-46AA13AD38C9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="398857568"/>
-        <c:axId val="398854288"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="398857568"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="398854288"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="398854288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="398857568"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Hyperbolic</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> normalized</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Tabelle1!$C$3:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>3.8747700143488543E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.12086042381097831</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.27487818347183435</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.55773000852456511</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0695388121807072</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.9843273365960763</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.6031966029837759</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.4451391286433379</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11.401713987690067</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-15AD-4CDE-8B7C-80460CEEC7B2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="398857568"/>
-        <c:axId val="398854288"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="398857568"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="398854288"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="398854288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="398857568"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -893,72 +235,72 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$23:$C$43</c:f>
+              <c:f>Tabelle1!$C$32:$C$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.130613194252668</c:v>
+                  <c:v>1.8393972058572117</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.3575888234288467</c:v>
+                  <c:v>0.67667641618306351</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.4626032029685962</c:v>
+                  <c:v>0.24893534183931973</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.706705664732254</c:v>
+                  <c:v>9.1578194443670893E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6416999724779759</c:v>
+                  <c:v>3.3689734995427337E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.99574136735727892</c:v>
+                  <c:v>1.2393760883331793E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.60394766844637005</c:v>
+                  <c:v>4.5594098277725809E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.36631277777468357</c:v>
+                  <c:v>1.6773131395125592E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.22217993076484613</c:v>
+                  <c:v>6.1704902043339775E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.13475893998170935</c:v>
+                  <c:v>2.2699964881242428E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.1735428769281332E-2</c:v>
+                  <c:v>8.3508503951228296E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.9575043533327173E-2</c:v>
+                  <c:v>3.072106176664105E-5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.0068783859551446E-2</c:v>
+                  <c:v>1.1301647034905271E-5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.8237639311090324E-2</c:v>
+                  <c:v>4.1576435955178392E-6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.1061687402956672E-2</c:v>
+                  <c:v>1.5295116025091289E-6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.7092525580502368E-3</c:v>
+                  <c:v>5.626758735962956E-7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.0693673802128837E-3</c:v>
+                  <c:v>2.0699688593925833E-7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.468196081733591E-3</c:v>
+                  <c:v>7.6149898723563142E-8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.4970365977540119E-3</c:v>
+                  <c:v>2.8013982187686337E-8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.0799859524969711E-4</c:v>
+                  <c:v>1.030576811219279E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1156,6 +498,854 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hyperbolic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$5:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$5:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>5.0694915703814311E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2687869338078004E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3452358160172736E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1806434778180287E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5162577716485961E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6242777937763291E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.8782722683361751E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.13693199373107739</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.20195531939442996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.27157166266833943</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.30559480084052726</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.27157166266833943</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.20195531939442996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13693199373107739</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.8782722683361751E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.6242777937763291E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.5162577716485961E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.1806434778180287E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.3452358160172736E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.2687869338078004E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.0694915703814311E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B2C1-4DF2-8BE1-E61900EAE384}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="710782200"/>
+        <c:axId val="710783184"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="710782200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="710783184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="710783184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="710782200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hyperbolic short</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$5:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$5:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>6.1027272741740034E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9540853051434692E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6194143319162562E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6250901579718863E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2329219623204989E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.7705869539551253E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.10687792566038574</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16484071454660576</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24311673443421419</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.32692189535175792</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.36787944117144233</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.32692189535175792</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.24311673443421419</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.16484071454660576</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.10687792566038574</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.7705869539551253E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.2329219623204989E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.6250901579718863E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.6194143319162562E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.9540853051434692E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.1027272741740034E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8CDE-4284-AF71-F98C2F7EC7D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="712490360"/>
+        <c:axId val="712490032"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="712490360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="712490032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="712490032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="712490360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2828,23 +3018,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>735330</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1">
+        <xdr:cNvPr id="4" name="Diagramm 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4885A909-7E6B-43DC-A0B1-FCD9EFAF390D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA80D837-224D-4FEF-9A03-F804A8DB7D4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2864,29 +3054,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2">
+        <xdr:cNvPr id="6" name="Diagramm 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A7D35D6-EE8E-48E9-B937-FB2D40D33DEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F31ADC08-CC00-4A9A-98B0-135FB65E8B52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2902,23 +3090,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Diagramm 3">
+        <xdr:cNvPr id="7" name="Diagramm 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA80D837-224D-4FEF-9A03-F804A8DB7D4C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF297E41-AC48-40D0-AA54-7033660F8BE9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3236,724 +3424,835 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409FB141-28C1-4A7F-8F52-AEC3C19D150B}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="1"/>
+    <col min="3" max="4" width="12" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="e">
-        <f>$G$7/(2*$G$4*$G$6*D18)*EXP(-$G$4*SQRT($G$6*$G$6+(A2-$G$3)*(A2-$G$3))+$G$5*(A2-$G$3))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D2" t="e">
-        <f t="shared" ref="D2:D12" si="0">BESSELK(A2,1)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <f>$G$7/(2*$G$4*$G$6*D3)*EXP(-$G$4*SQRT($G$6*$G$6+(A3-$G$3)*(A3-$G$3))+$G$5*(A3-$G$3))</f>
-        <v>0.28835877333528559</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C12" si="1">B3/$B$14*$G$2</f>
-        <v>3.8747700143488543E-2</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>0.60190723166690574</v>
-      </c>
-      <c r="F3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <f t="shared" ref="B4:B12" si="2">$G$7/(2*$G$4*$G$6*D4)*EXP(-$G$4*SQRT($G$6*$G$6+(A4-$G$3)*(A4-$G$3))+$G$5*(A4-$G$3))</f>
-        <v>0.89943824861494659</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="1"/>
-        <v>0.12086042381097831</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.13986588</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <f t="shared" si="2"/>
-        <v>2.0456320119399338</v>
+        <f>$F$9/(2*$F$5*$F$7*$F$10)*EXP($F$6*(A5-$F$4)-$F$5*SQRT($F$7*$F$7+(A5-$F$4)*(A5-$F$4)))</f>
+        <v>5.0694915703814311E-3</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
-        <v>0.27487818347183435</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>4.0156431243917462E-2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.5</v>
+        <f>EXP($F$6*(A5-$F$4)-$F$5*SQRT($F$7*$F$7+(A5-$F$4)*(A5-$F$4)))</f>
+        <v>6.1027272741740034E-3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="B6">
-        <f t="shared" si="2"/>
-        <v>4.1506035329802264</v>
+        <f t="shared" ref="B6:B25" si="0">$F$9/(2*$F$5*$F$7*$F$10)*EXP($F$6*(A6-$F$4)-$F$5*SQRT($F$7*$F$7+(A6-$F$4)*(A6-$F$4)))</f>
+        <v>8.2687869338078004E-3</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
-        <v>0.55773000852456511</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>1.2483498888160477E-2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
+        <f t="shared" ref="C6:C25" si="1">EXP($F$6*(A6-$F$4)-$F$5*SQRT($F$7*$F$7+(A6-$F$4)*(A6-$F$4)))</f>
+        <v>9.9540853051434692E-3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <f t="shared" si="2"/>
-        <v>7.9594633687371203</v>
+        <f t="shared" si="0"/>
+        <v>1.3452358160172736E-2</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>1.0695388121807072</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>4.044613383208274E-3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="1">
-        <f>SQRT(G4*G4-G5*G5)</f>
-        <v>0.8660254037844386</v>
+        <v>1.6194143319162562E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="B8">
-        <f t="shared" si="2"/>
-        <v>14.767281530454278</v>
+        <f t="shared" si="0"/>
+        <v>2.1806434778180287E-2</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>1.9843273365960763</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1.3439197167432592E-3</v>
-      </c>
+        <v>2.6250901579718863E-2</v>
+      </c>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <f t="shared" si="2"/>
-        <v>26.814839298194407</v>
+        <f t="shared" si="0"/>
+        <v>3.5162577716485961E-2</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>3.6031966029837759</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>4.5418249556302272E-4</v>
+        <v>4.2329219623204989E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1">
+        <f>SQRT($F$5*$F$5-$F$6*$F$6)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="B10">
-        <f t="shared" si="2"/>
-        <v>47.964457405949112</v>
+        <f t="shared" si="0"/>
+        <v>5.6242777937763291E-2</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>6.4451391286433379</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>1.5536921660488915E-4</v>
+        <v>6.7705869539551253E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f>BESSELK($F$7*$F$9,1)</f>
+        <v>0.60190723166690574</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <f t="shared" si="2"/>
-        <v>84.851081412184911</v>
+        <f t="shared" si="0"/>
+        <v>8.8782722683361751E-2</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>11.401713987690067</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>5.3637018130208138E-5</v>
+        <v>0.10687792566038574</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>10</v>
+        <v>3.5</v>
       </c>
       <c r="B12">
-        <f t="shared" si="2"/>
-        <v>148.83916839835646</v>
+        <f t="shared" si="0"/>
+        <v>0.13693199373107739</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="D12">
+        <v>0.16484071454660576</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
         <f t="shared" si="0"/>
-        <v>1.8648773946849075E-5</v>
+        <v>0.20195531939442996</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0.24311673443421419</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14">
+        <v>4.5</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0.27157166266833943</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>0.32692189535175792</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0.30559480084052726</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.36787944117144233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>5.5</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0.27157166266833943</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.32692189535175792</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0.20195531939442996</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.24311673443421419</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>6.5</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0.13693199373107739</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0.16484071454660576</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>8.8782722683361751E-2</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>0.10687792566038574</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>7.5</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>5.6242777937763291E-2</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>6.7705869539551253E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>8</v>
       </c>
-      <c r="B14">
-        <f>MAX(B3:B12)</f>
-        <v>148.83916839835646</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20">
-        <v>0.5</v>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>3.5162577716485961E-2</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>4.2329219623204989E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>8.5</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>2.1806434778180287E-2</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>2.6250901579718863E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>1.3452358160172736E-2</v>
       </c>
       <c r="C23">
-        <f>$G$2*EXP(-$B$20*A23)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>1.6194143319162562E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>1</v>
+        <v>9.5</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>8.2687869338078004E-3</v>
       </c>
       <c r="C24">
-        <f t="shared" ref="C24:C73" si="3">$G$2*EXP(-$B$20*A24)</f>
-        <v>12.130613194252668</v>
+        <f t="shared" si="1"/>
+        <v>9.9540853051434692E-3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>5.0694915703814311E-3</v>
       </c>
       <c r="C25">
-        <f t="shared" si="3"/>
-        <v>7.3575888234288467</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="3"/>
-        <v>4.4626032029685962</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>4</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="3"/>
-        <v>2.706705664732254</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>6.1027272741740034E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>5</v>
       </c>
-      <c r="C28">
-        <f t="shared" si="3"/>
-        <v>1.6416999724779759</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="B30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>6</v>
       </c>
-      <c r="C29">
-        <f t="shared" si="3"/>
-        <v>0.99574136735727892</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>7</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="3"/>
-        <v>0.60394766844637005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>8</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="3"/>
-        <v>0.36631277777468357</v>
+      <c r="B31">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="3"/>
-        <v>0.22217993076484613</v>
+        <f>$B$30*EXP(-$B$31*A32)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <f t="shared" si="3"/>
-        <v>0.13475893998170935</v>
+        <f>$B$30*EXP(-$B$31*A33)</f>
+        <v>1.8393972058572117</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <f t="shared" si="3"/>
-        <v>8.1735428769281332E-2</v>
+        <f>$B$30*EXP(-$B$31*A34)</f>
+        <v>0.67667641618306351</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C35">
-        <f t="shared" si="3"/>
-        <v>4.9575043533327173E-2</v>
+        <f>$B$30*EXP(-$B$31*A35)</f>
+        <v>0.24893534183931973</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C36">
-        <f t="shared" si="3"/>
-        <v>3.0068783859551446E-2</v>
+        <f>$B$30*EXP(-$B$31*A36)</f>
+        <v>9.1578194443670893E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C37">
-        <f t="shared" si="3"/>
-        <v>1.8237639311090324E-2</v>
+        <f>$B$30*EXP(-$B$31*A37)</f>
+        <v>3.3689734995427337E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C38">
-        <f t="shared" si="3"/>
-        <v>1.1061687402956672E-2</v>
+        <f>$B$30*EXP(-$B$31*A38)</f>
+        <v>1.2393760883331793E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C39">
-        <f t="shared" si="3"/>
-        <v>6.7092525580502368E-3</v>
+        <f>$B$30*EXP(-$B$31*A39)</f>
+        <v>4.5594098277725809E-3</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C40">
-        <f t="shared" si="3"/>
-        <v>4.0693673802128837E-3</v>
+        <f>$B$30*EXP(-$B$31*A40)</f>
+        <v>1.6773131395125592E-3</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C41">
-        <f t="shared" si="3"/>
-        <v>2.468196081733591E-3</v>
+        <f>$B$30*EXP(-$B$31*A41)</f>
+        <v>6.1704902043339775E-4</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C42">
-        <f t="shared" si="3"/>
-        <v>1.4970365977540119E-3</v>
+        <f>$B$30*EXP(-$B$31*A42)</f>
+        <v>2.2699964881242428E-4</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C43">
-        <f t="shared" si="3"/>
-        <v>9.0799859524969711E-4</v>
+        <f>$B$30*EXP(-$B$31*A43)</f>
+        <v>8.3508503951228296E-5</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C44">
-        <f t="shared" si="3"/>
-        <v>5.5072898699494314E-4</v>
+        <f>$B$30*EXP(-$B$31*A44)</f>
+        <v>3.072106176664105E-5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C45">
-        <f t="shared" si="3"/>
-        <v>3.3403401580491319E-4</v>
+        <f>$B$30*EXP(-$B$31*A45)</f>
+        <v>1.1301647034905271E-5</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C46">
-        <f t="shared" si="3"/>
-        <v>2.0260187197261421E-4</v>
+        <f>$B$30*EXP(-$B$31*A46)</f>
+        <v>4.1576435955178392E-6</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C47">
-        <f t="shared" si="3"/>
-        <v>1.228842470665642E-4</v>
+        <f>$B$30*EXP(-$B$31*A47)</f>
+        <v>1.5295116025091289E-6</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C48">
-        <f t="shared" si="3"/>
-        <v>7.4533063441573419E-5</v>
+        <f>$B$30*EXP(-$B$31*A48)</f>
+        <v>5.626758735962956E-7</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C49">
-        <f t="shared" si="3"/>
-        <v>4.5206588139621085E-5</v>
+        <f>$B$30*EXP(-$B$31*A49)</f>
+        <v>2.0699688593925833E-7</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C50">
-        <f t="shared" si="3"/>
-        <v>2.741918172768169E-5</v>
+        <f>$B$30*EXP(-$B$31*A50)</f>
+        <v>7.6149898723563142E-8</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C51">
-        <f t="shared" si="3"/>
-        <v>1.6630574382071357E-5</v>
+        <f>$B$30*EXP(-$B$31*A51)</f>
+        <v>2.8013982187686337E-8</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C52">
-        <f t="shared" si="3"/>
-        <v>1.0086953251357761E-5</v>
+        <f>$B$30*EXP(-$B$31*A52)</f>
+        <v>1.030576811219279E-8</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C53">
-        <f t="shared" si="3"/>
-        <v>6.1180464100365157E-6</v>
+        <f>$B$30*EXP(-$B$31*A53)</f>
+        <v>3.7912802139559537E-9</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C54">
-        <f t="shared" si="3"/>
-        <v>3.7107827252319566E-6</v>
+        <f>$B$30*EXP(-$B$31*A54)</f>
+        <v>1.3947340464344622E-9</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C55">
-        <f t="shared" si="3"/>
-        <v>2.2507034943851824E-6</v>
+        <f>$B$30*EXP(-$B$31*A55)</f>
+        <v>5.1309398158509455E-10</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C56">
-        <f t="shared" si="3"/>
-        <v>1.365120675266974E-6</v>
+        <f>$B$30*EXP(-$B$31*A56)</f>
+        <v>1.8875672721395487E-10</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C57">
-        <f t="shared" si="3"/>
-        <v>8.2798754375703334E-7</v>
+        <f>$B$30*EXP(-$B$31*A57)</f>
+        <v>6.9439719324820108E-11</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C58">
-        <f t="shared" si="3"/>
-        <v>5.0219983114879633E-7</v>
+        <f>$B$30*EXP(-$B$31*A58)</f>
+        <v>2.5545445140316624E-11</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C59">
-        <f t="shared" si="3"/>
-        <v>3.0459959489425257E-7</v>
+        <f>$B$30*EXP(-$B$31*A59)</f>
+        <v>9.3976440826954154E-12</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C60">
-        <f t="shared" si="3"/>
-        <v>1.8474899323941189E-7</v>
+        <f>$B$30*EXP(-$B$31*A60)</f>
+        <v>3.4572000534701013E-12</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C61">
-        <f t="shared" si="3"/>
-        <v>1.1205592875074535E-7</v>
+        <f>$B$30*EXP(-$B$31*A61)</f>
+        <v>1.2718328236884614E-12</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C62">
-        <f t="shared" si="3"/>
-        <v>6.7965356389901423E-8</v>
+        <f>$B$30*EXP(-$B$31*A62)</f>
+        <v>4.6788114844200873E-13</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C63">
-        <f t="shared" si="3"/>
-        <v>4.1223072448771159E-8</v>
+        <f>$B$30*EXP(-$B$31*A63)</f>
+        <v>1.7212385542349882E-13</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C64">
-        <f t="shared" si="3"/>
-        <v>2.5003057327734852E-8</v>
+        <f>$B$30*EXP(-$B$31*A64)</f>
+        <v>6.3320827745470878E-14</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C65">
-        <f t="shared" si="3"/>
-        <v>1.5165120855823815E-8</v>
+        <f>$B$30*EXP(-$B$31*A65)</f>
+        <v>2.3294430725516989E-14</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C66">
-        <f t="shared" si="3"/>
-        <v>9.1981107573046339E-9</v>
+        <f>$B$30*EXP(-$B$31*A66)</f>
+        <v>8.569542157710065E-15</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C67">
-        <f t="shared" si="3"/>
-        <v>5.5789361857378489E-9</v>
+        <f>$B$30*EXP(-$B$31*A67)</f>
+        <v>3.1525583800734946E-15</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C68">
-        <f t="shared" si="3"/>
-        <v>3.3837958452302609E-9</v>
+        <f>$B$30*EXP(-$B$31*A68)</f>
+        <v>1.1597614151217846E-15</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C69">
-        <f t="shared" si="3"/>
-        <v>2.0523759263403782E-9</v>
+        <f>$B$30*EXP(-$B$31*A69)</f>
+        <v>4.2665238128720328E-16</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C70">
-        <f t="shared" si="3"/>
-        <v>1.2448289245815564E-9</v>
+        <f>$B$30*EXP(-$B$31*A70)</f>
+        <v>1.5695663960240149E-16</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C71">
-        <f t="shared" si="3"/>
-        <v>7.5502690885581949E-10</v>
+        <f>$B$30*EXP(-$B$31*A71)</f>
+        <v>5.7741120865078931E-17</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C72">
-        <f t="shared" si="3"/>
-        <v>4.579469691291106E-10</v>
+        <f>$B$30*EXP(-$B$31*A72)</f>
+        <v>2.1241771276457944E-17</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
+        <v>41</v>
+      </c>
+      <c r="C73">
+        <f>$B$30*EXP(-$B$31*A73)</f>
+        <v>7.814410946674944E-18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>42</v>
+      </c>
+      <c r="C74">
+        <f>$B$30*EXP(-$B$31*A74)</f>
+        <v>2.8747611321467799E-18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>43</v>
+      </c>
+      <c r="C75">
+        <f>$B$30*EXP(-$B$31*A75)</f>
+        <v>1.0575655187955403E-18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>44</v>
+      </c>
+      <c r="C76">
+        <f>$B$30*EXP(-$B$31*A76)</f>
+        <v>3.8905661205668983E-19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>45</v>
+      </c>
+      <c r="C77">
+        <f>$B$30*EXP(-$B$31*A77)</f>
+        <v>1.4312592902746968E-19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>46</v>
+      </c>
+      <c r="C78">
+        <f>$B$30*EXP(-$B$31*A78)</f>
+        <v>5.2653086787769062E-20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>47</v>
+      </c>
+      <c r="C79">
+        <f>$B$30*EXP(-$B$31*A79)</f>
+        <v>1.9369988143435932E-20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>48</v>
+      </c>
+      <c r="C80">
+        <f>$B$30*EXP(-$B$31*A80)</f>
+        <v>7.1258204137046756E-21</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>49</v>
+      </c>
+      <c r="C81">
+        <f>$B$30*EXP(-$B$31*A81)</f>
+        <v>2.6214428316817319E-21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82">
         <v>50</v>
       </c>
-      <c r="C73">
-        <f t="shared" si="3"/>
-        <v>2.7775887729928043E-10</v>
+      <c r="C82">
+        <f>$B$30*EXP(-$B$31*A82)</f>
+        <v>9.6437492398195884E-22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>